<commit_message>
created sprint backlog sheet
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Management Tool" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Tasks</t>
     <phoneticPr fontId="1"/>
@@ -61,6 +62,58 @@
   </si>
   <si>
     <t>6.1 Get (merged) columns of current date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TO DO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DONE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Invoke macros either by clicking a button, when data changes, or when workbook is opened</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Refresh pivot tables and pivot charts </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Get last Friday and current Thursday</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Change title of pivot chart</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Set pivot table filter based on current week (Fri start)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Get (merged) columns of current date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read data from external workbooks by input box</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read and accumulate data from Anken rows</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read and accumulate data from non-Anken rows</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Add data to source worksheet</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -93,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +156,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,13 +178,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,75 +498,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="26.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27" x14ac:dyDescent="0.15">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -513,4 +578,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.75" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moved tasks to done and added new tasks
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Progress Management Tool" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Tasks</t>
     <phoneticPr fontId="1"/>
@@ -114,6 +114,38 @@
   </si>
   <si>
     <t>Add data to source worksheet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Include naibu kadai hours (which is under Z common) to anken data</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify addition of data to source worksheet </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read and accumulate anken data from last Friday to current Thursday from each 作業実績 file</t>
+    <rPh sb="78" eb="80">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t>ジッセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read and accumulate non-anken data from last Friday to current Thursday from each 作業実績 file</t>
+    <rPh sb="82" eb="84">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>ジッセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Modify date filter to allow users to set date range of  date filter</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -584,10 +616,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -645,18 +677,43 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>